<commit_message>
Update supply and demand data
</commit_message>
<xml_diff>
--- a/epm/input/data_capp/load/pDemandForecast.xlsx
+++ b/epm/input/data_capp/load/pDemandForecast.xlsx
@@ -8,24 +8,37 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucas/Documents/World Bank/Projects/EPM_APPLIED/EPM_CAPP/epm/input/data_capp/load/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5AFF22B-DC48-DD47-A4E1-F849C12FD6E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54FF4C77-70EA-1641-A1B9-4F643D99C871}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="1820" windowWidth="25800" windowHeight="16440" activeTab="1" xr2:uid="{C2E2233B-F7F2-434F-AE42-307C2775D8C3}"/>
+    <workbookView xWindow="10520" yWindow="1380" windowWidth="25800" windowHeight="16440" activeTab="1" xr2:uid="{C2E2233B-F7F2-434F-AE42-307C2775D8C3}"/>
   </bookViews>
   <sheets>
     <sheet name="pDemandForecast" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7853" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7854" uniqueCount="43">
   <si>
     <t>zone</t>
   </si>
@@ -153,7 +166,7 @@
     <t>Grand Total</t>
   </si>
   <si>
-    <t>Sum of ene_demandElectrical Energy Demand (GWh)</t>
+    <t>Sum of Peak Load Demand (MW)</t>
   </si>
 </sst>
 </file>
@@ -696,7 +709,91 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="34">
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
@@ -16385,7 +16482,7 @@
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{416D3396-C041-824F-B5AF-4A577129E5CB}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" showDrill="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" showHeaders="0" compact="0" compactData="0" multipleFieldFilters="0">
-  <location ref="A3:V15" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <location ref="A3:V16" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="10">
     <pivotField compact="0" outline="0" showAll="0"/>
     <pivotField axis="axisCol" compact="0" outline="0" showAll="0">
@@ -16430,15 +16527,15 @@
         <item t="default"/>
       </items>
     </pivotField>
+    <pivotField compact="0" outline="0" showAll="0"/>
     <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
     <pivotField compact="0" outline="0" showAll="0"/>
     <pivotField compact="0" outline="0" showAll="0"/>
     <pivotField axis="axisPage" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0">
       <items count="7">
         <item h="1" x="0"/>
-        <item x="1"/>
-        <item h="1" x="3"/>
+        <item h="1" x="1"/>
+        <item x="3"/>
         <item h="1" x="4"/>
         <item h="1" x="5"/>
         <item h="1" x="2"/>
@@ -16451,7 +16548,7 @@
   <rowFields count="1">
     <field x="2"/>
   </rowFields>
-  <rowItems count="11">
+  <rowItems count="12">
     <i>
       <x/>
     </i>
@@ -16471,7 +16568,7 @@
       <x v="5"/>
     </i>
     <i>
-      <x v="6"/>
+      <x v="7"/>
     </i>
     <i>
       <x v="8"/>
@@ -16481,6 +16578,9 @@
     </i>
     <i>
       <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
     </i>
     <i t="grand">
       <x/>
@@ -16558,10 +16658,10 @@
     <pageField fld="7" hier="-1"/>
   </pageFields>
   <dataFields count="1">
-    <dataField name="Sum of ene_demandElectrical Energy Demand (GWh)" fld="3" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Peak Load Demand (MW)" fld="4" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="5">
+    <format dxfId="33">
       <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="2" count="11" selected="0">
@@ -16580,7 +16680,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="4">
+    <format dxfId="32">
       <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="2" count="11" selected="0">
@@ -18502,17 +18602,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ADB6FE6-D7D6-0D47-A0B4-36610526AE39}">
-  <dimension ref="A1:V15"/>
+  <dimension ref="A1:V16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="57" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="48.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="21" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="21" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="23" max="41" width="48.1640625" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="52.83203125" bestFit="1" customWidth="1"/>
     <col min="43" max="43" width="33.83203125" bestFit="1" customWidth="1"/>
@@ -18609,7 +18709,7 @@
         <v>22</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.2">
@@ -18687,67 +18787,67 @@
         <v>2</v>
       </c>
       <c r="B5" s="3">
-        <v>7833</v>
+        <v>2298</v>
       </c>
       <c r="C5" s="3">
-        <v>8299</v>
+        <v>2405</v>
       </c>
       <c r="D5" s="3">
-        <v>8764.34</v>
+        <v>2520</v>
       </c>
       <c r="E5" s="3">
-        <v>9230</v>
+        <v>2642</v>
       </c>
       <c r="F5" s="3">
-        <v>9696</v>
+        <v>2774</v>
       </c>
       <c r="G5" s="3">
-        <v>10118.959999999999</v>
+        <v>2915</v>
       </c>
       <c r="H5" s="3">
-        <v>10542.13</v>
+        <v>3066</v>
       </c>
       <c r="I5" s="3">
-        <v>10965</v>
+        <v>3228</v>
       </c>
       <c r="J5" s="3">
-        <v>11388</v>
+        <v>3401</v>
       </c>
       <c r="K5" s="3">
-        <v>11811.65</v>
+        <v>3586</v>
       </c>
       <c r="L5" s="3">
-        <v>12262.73</v>
+        <v>3785</v>
       </c>
       <c r="M5" s="3">
-        <v>12714</v>
+        <v>3998</v>
       </c>
       <c r="N5" s="3">
-        <v>13165</v>
+        <v>4227</v>
       </c>
       <c r="O5" s="3">
-        <v>13616</v>
+        <v>4471</v>
       </c>
       <c r="P5" s="3">
-        <v>14067.03</v>
+        <v>4733</v>
       </c>
       <c r="Q5" s="3">
-        <v>14555</v>
+        <v>5014</v>
       </c>
       <c r="R5" s="3">
-        <v>15044</v>
+        <v>5314</v>
       </c>
       <c r="S5" s="3">
-        <v>15531.86</v>
+        <v>5637</v>
       </c>
       <c r="T5" s="3">
-        <v>16020</v>
+        <v>5982</v>
       </c>
       <c r="U5" s="3">
-        <v>16508.41</v>
+        <v>6351</v>
       </c>
       <c r="V5" s="3">
-        <v>242132.11000000002</v>
+        <v>78347</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.2">
@@ -18755,67 +18855,67 @@
         <v>4</v>
       </c>
       <c r="B6" s="3">
-        <v>382</v>
+        <v>79</v>
       </c>
       <c r="C6" s="3">
-        <v>407</v>
+        <v>87</v>
       </c>
       <c r="D6" s="3">
-        <v>431.4</v>
+        <v>96</v>
       </c>
       <c r="E6" s="3">
-        <v>456</v>
+        <v>105</v>
       </c>
       <c r="F6" s="3">
-        <v>481</v>
+        <v>115</v>
       </c>
       <c r="G6" s="3">
-        <v>509.6</v>
+        <v>126</v>
       </c>
       <c r="H6" s="3">
-        <v>538.20000000000005</v>
+        <v>139</v>
       </c>
       <c r="I6" s="3">
-        <v>567</v>
+        <v>152</v>
       </c>
       <c r="J6" s="3">
-        <v>595</v>
+        <v>167</v>
       </c>
       <c r="K6" s="3">
-        <v>624</v>
+        <v>184</v>
       </c>
       <c r="L6" s="3">
-        <v>647.53</v>
+        <v>201</v>
       </c>
       <c r="M6" s="3">
-        <v>675</v>
+        <v>221</v>
       </c>
       <c r="N6" s="3">
-        <v>702</v>
+        <v>243</v>
       </c>
       <c r="O6" s="3">
-        <v>728</v>
+        <v>266</v>
       </c>
       <c r="P6" s="3">
-        <v>755.48</v>
+        <v>292</v>
       </c>
       <c r="Q6" s="3">
-        <v>782</v>
+        <v>321</v>
       </c>
       <c r="R6" s="3">
-        <v>809</v>
+        <v>352</v>
       </c>
       <c r="S6" s="3">
-        <v>836.45</v>
+        <v>387</v>
       </c>
       <c r="T6" s="3">
-        <v>863</v>
+        <v>424</v>
       </c>
       <c r="U6" s="3">
-        <v>890.42</v>
+        <v>466</v>
       </c>
       <c r="V6" s="3">
-        <v>12680.08</v>
+        <v>4423</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.2">
@@ -18823,67 +18923,67 @@
         <v>5</v>
       </c>
       <c r="B7" s="3">
-        <v>9171</v>
+        <v>1291</v>
       </c>
       <c r="C7" s="3">
-        <v>9716</v>
+        <v>1399</v>
       </c>
       <c r="D7" s="3">
-        <v>10261.76</v>
+        <v>1517</v>
       </c>
       <c r="E7" s="3">
-        <v>10807</v>
+        <v>1645</v>
       </c>
       <c r="F7" s="3">
-        <v>11352</v>
+        <v>1784</v>
       </c>
       <c r="G7" s="3">
-        <v>11847.83</v>
+        <v>1934</v>
       </c>
       <c r="H7" s="3">
-        <v>12343.3</v>
+        <v>2098</v>
       </c>
       <c r="I7" s="3">
-        <v>12839</v>
+        <v>2275</v>
       </c>
       <c r="J7" s="3">
-        <v>13334</v>
+        <v>2466</v>
       </c>
       <c r="K7" s="3">
-        <v>13829.72</v>
+        <v>2674</v>
       </c>
       <c r="L7" s="3">
-        <v>14357.87</v>
+        <v>2900</v>
       </c>
       <c r="M7" s="3">
-        <v>14886</v>
+        <v>3144</v>
       </c>
       <c r="N7" s="3">
-        <v>15414</v>
+        <v>3410</v>
       </c>
       <c r="O7" s="3">
-        <v>15942</v>
+        <v>3697</v>
       </c>
       <c r="P7" s="3">
-        <v>16470.439999999999</v>
+        <v>4009</v>
       </c>
       <c r="Q7" s="3">
-        <v>17042</v>
+        <v>4347</v>
       </c>
       <c r="R7" s="3">
-        <v>17614</v>
+        <v>4713</v>
       </c>
       <c r="S7" s="3">
-        <v>18185.54</v>
+        <v>5111</v>
       </c>
       <c r="T7" s="3">
-        <v>18757</v>
+        <v>5542</v>
       </c>
       <c r="U7" s="3">
-        <v>19328.95</v>
+        <v>6009</v>
       </c>
       <c r="V7" s="3">
-        <v>283499.40999999997</v>
+        <v>61965</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.2">
@@ -18891,67 +18991,67 @@
         <v>36</v>
       </c>
       <c r="B8" s="3">
-        <v>92</v>
+        <v>13</v>
       </c>
       <c r="C8" s="3">
-        <v>97</v>
+        <v>14</v>
       </c>
       <c r="D8" s="3">
-        <v>102.76</v>
+        <v>16</v>
       </c>
       <c r="E8" s="3">
-        <v>108</v>
+        <v>18</v>
       </c>
       <c r="F8" s="3">
+        <v>20</v>
+      </c>
+      <c r="G8" s="3">
+        <v>23</v>
+      </c>
+      <c r="H8" s="3">
+        <v>26</v>
+      </c>
+      <c r="I8" s="3">
+        <v>29</v>
+      </c>
+      <c r="J8" s="3">
+        <v>33</v>
+      </c>
+      <c r="K8" s="3">
+        <v>38</v>
+      </c>
+      <c r="L8" s="3">
+        <v>44</v>
+      </c>
+      <c r="M8" s="3">
+        <v>50</v>
+      </c>
+      <c r="N8" s="3">
+        <v>56</v>
+      </c>
+      <c r="O8" s="3">
+        <v>64</v>
+      </c>
+      <c r="P8" s="3">
+        <v>72</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>81</v>
+      </c>
+      <c r="R8" s="3">
+        <v>91</v>
+      </c>
+      <c r="S8" s="3">
+        <v>102</v>
+      </c>
+      <c r="T8" s="3">
         <v>114</v>
       </c>
-      <c r="G8" s="3">
-        <v>118.65</v>
-      </c>
-      <c r="H8" s="3">
-        <v>123.61</v>
-      </c>
-      <c r="I8" s="3">
-        <v>129</v>
-      </c>
-      <c r="J8" s="3">
-        <v>134</v>
-      </c>
-      <c r="K8" s="3">
-        <v>138.5</v>
-      </c>
-      <c r="L8" s="3">
-        <v>143.78</v>
-      </c>
-      <c r="M8" s="3">
-        <v>149</v>
-      </c>
-      <c r="N8" s="3">
-        <v>154</v>
-      </c>
-      <c r="O8" s="3">
-        <v>160</v>
-      </c>
-      <c r="P8" s="3">
-        <v>164.94</v>
-      </c>
-      <c r="Q8" s="3">
-        <v>171</v>
-      </c>
-      <c r="R8" s="3">
-        <v>176</v>
-      </c>
-      <c r="S8" s="3">
-        <v>182.12</v>
-      </c>
-      <c r="T8" s="3">
-        <v>188</v>
-      </c>
       <c r="U8" s="3">
-        <v>193.57</v>
+        <v>127</v>
       </c>
       <c r="V8" s="3">
-        <v>2839.93</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.2">
@@ -18959,67 +19059,67 @@
         <v>7</v>
       </c>
       <c r="B9" s="3">
-        <v>524</v>
+        <v>59</v>
       </c>
       <c r="C9" s="3">
-        <v>278</v>
+        <v>64</v>
       </c>
       <c r="D9" s="3">
-        <v>293.61</v>
+        <v>69</v>
       </c>
       <c r="E9" s="3">
-        <v>309</v>
+        <v>74</v>
       </c>
       <c r="F9" s="3">
-        <v>325</v>
+        <v>81</v>
       </c>
       <c r="G9" s="3">
-        <v>338.99</v>
+        <v>89</v>
       </c>
       <c r="H9" s="3">
-        <v>353.17</v>
+        <v>98</v>
       </c>
       <c r="I9" s="3">
-        <v>367</v>
+        <v>108</v>
       </c>
       <c r="J9" s="3">
-        <v>382</v>
+        <v>119</v>
       </c>
       <c r="K9" s="3">
-        <v>395.7</v>
+        <v>132</v>
       </c>
       <c r="L9" s="3">
-        <v>410.81</v>
+        <v>146</v>
       </c>
       <c r="M9" s="3">
-        <v>426</v>
+        <v>161</v>
       </c>
       <c r="N9" s="3">
-        <v>441</v>
+        <v>177</v>
       </c>
       <c r="O9" s="3">
-        <v>456</v>
+        <v>195</v>
       </c>
       <c r="P9" s="3">
-        <v>471.26</v>
+        <v>214</v>
       </c>
       <c r="Q9" s="3">
-        <v>488</v>
+        <v>235</v>
       </c>
       <c r="R9" s="3">
-        <v>504</v>
+        <v>257</v>
       </c>
       <c r="S9" s="3">
-        <v>520.33000000000004</v>
+        <v>280</v>
       </c>
       <c r="T9" s="3">
-        <v>537</v>
+        <v>306</v>
       </c>
       <c r="U9" s="3">
-        <v>553.04999999999995</v>
+        <v>333</v>
       </c>
       <c r="V9" s="3">
-        <v>8373.92</v>
+        <v>3197</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.2">
@@ -19027,135 +19127,135 @@
         <v>8</v>
       </c>
       <c r="B10" s="3">
-        <v>2112</v>
+        <v>448</v>
       </c>
       <c r="C10" s="3">
-        <v>2238</v>
+        <v>472</v>
       </c>
       <c r="D10" s="3">
-        <v>2363.58</v>
+        <v>496</v>
       </c>
       <c r="E10" s="3">
-        <v>2489</v>
+        <v>522</v>
       </c>
       <c r="F10" s="3">
-        <v>2615</v>
+        <v>549</v>
       </c>
       <c r="G10" s="3">
-        <v>2728.9</v>
+        <v>578</v>
       </c>
       <c r="H10" s="3">
-        <v>2843.02</v>
+        <v>608</v>
       </c>
       <c r="I10" s="3">
-        <v>2957</v>
+        <v>640</v>
       </c>
       <c r="J10" s="3">
-        <v>3071</v>
+        <v>674</v>
       </c>
       <c r="K10" s="3">
-        <v>3185.39</v>
+        <v>709</v>
       </c>
       <c r="L10" s="3">
-        <v>3307.03</v>
+        <v>746</v>
       </c>
       <c r="M10" s="3">
-        <v>3429</v>
+        <v>785</v>
       </c>
       <c r="N10" s="3">
-        <v>3550</v>
+        <v>826</v>
       </c>
       <c r="O10" s="3">
-        <v>3672</v>
+        <v>869</v>
       </c>
       <c r="P10" s="3">
-        <v>3793.62</v>
+        <v>914</v>
       </c>
       <c r="Q10" s="3">
-        <v>3925</v>
+        <v>962</v>
       </c>
       <c r="R10" s="3">
-        <v>4057</v>
+        <v>1012</v>
       </c>
       <c r="S10" s="3">
-        <v>4188.66</v>
+        <v>1065</v>
       </c>
       <c r="T10" s="3">
-        <v>4320</v>
+        <v>1121</v>
       </c>
       <c r="U10" s="3">
-        <v>4452.0200000000004</v>
+        <v>1180</v>
       </c>
       <c r="V10" s="3">
-        <v>65297.22</v>
+        <v>15176</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11" s="3">
-        <v>9788</v>
-      </c>
-      <c r="C11" s="3">
-        <v>10370</v>
-      </c>
-      <c r="D11" s="3">
-        <v>10951.75</v>
-      </c>
-      <c r="E11" s="3">
-        <v>11534</v>
-      </c>
-      <c r="F11" s="3">
-        <v>12116</v>
-      </c>
-      <c r="G11" s="3">
-        <v>12644.46</v>
-      </c>
-      <c r="H11" s="3">
-        <v>13173.25</v>
-      </c>
-      <c r="I11" s="3">
-        <v>13702</v>
-      </c>
-      <c r="J11" s="3">
-        <v>14231</v>
-      </c>
-      <c r="K11" s="3">
-        <v>14759.62</v>
-      </c>
-      <c r="L11" s="3">
-        <v>15323.27</v>
-      </c>
-      <c r="M11" s="3">
-        <v>15887</v>
-      </c>
-      <c r="N11" s="3">
-        <v>16451</v>
-      </c>
-      <c r="O11" s="3">
-        <v>17014</v>
-      </c>
-      <c r="P11" s="3">
-        <v>17577.89</v>
-      </c>
-      <c r="Q11" s="3">
-        <v>18188</v>
-      </c>
-      <c r="R11" s="3">
-        <v>18798</v>
-      </c>
-      <c r="S11" s="3">
-        <v>19408.32</v>
-      </c>
-      <c r="T11" s="3">
-        <v>20018</v>
-      </c>
-      <c r="U11" s="3">
-        <v>20628.599999999999</v>
-      </c>
-      <c r="V11" s="3">
-        <v>302564.15999999997</v>
+        <v>38</v>
+      </c>
+      <c r="B11" s="4">
+        <v>1808</v>
+      </c>
+      <c r="C11" s="4">
+        <v>1962</v>
+      </c>
+      <c r="D11" s="4">
+        <v>2130</v>
+      </c>
+      <c r="E11" s="4">
+        <v>2312</v>
+      </c>
+      <c r="F11" s="4">
+        <v>2509</v>
+      </c>
+      <c r="G11" s="4">
+        <v>2723</v>
+      </c>
+      <c r="H11" s="4">
+        <v>2955</v>
+      </c>
+      <c r="I11" s="4">
+        <v>3208</v>
+      </c>
+      <c r="J11" s="4">
+        <v>3481</v>
+      </c>
+      <c r="K11" s="4">
+        <v>3778</v>
+      </c>
+      <c r="L11" s="4">
+        <v>4055</v>
+      </c>
+      <c r="M11" s="4">
+        <v>4336</v>
+      </c>
+      <c r="N11" s="4">
+        <v>4615</v>
+      </c>
+      <c r="O11" s="4">
+        <v>4843</v>
+      </c>
+      <c r="P11" s="4">
+        <v>5073</v>
+      </c>
+      <c r="Q11" s="4">
+        <v>5242</v>
+      </c>
+      <c r="R11" s="4">
+        <v>5423</v>
+      </c>
+      <c r="S11" s="4">
+        <v>5605</v>
+      </c>
+      <c r="T11" s="4">
+        <v>5786</v>
+      </c>
+      <c r="U11" s="4">
+        <v>5968</v>
+      </c>
+      <c r="V11" s="4">
+        <v>77812</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.2">
@@ -19163,67 +19263,67 @@
         <v>39</v>
       </c>
       <c r="B12" s="3">
-        <v>611</v>
+        <v>108</v>
       </c>
       <c r="C12" s="3">
-        <v>648</v>
+        <v>133</v>
       </c>
       <c r="D12" s="3">
-        <v>684.12</v>
+        <v>164</v>
       </c>
       <c r="E12" s="3">
-        <v>720</v>
+        <v>202</v>
       </c>
       <c r="F12" s="3">
-        <v>757</v>
+        <v>248</v>
       </c>
       <c r="G12" s="3">
-        <v>789.86</v>
+        <v>306</v>
       </c>
       <c r="H12" s="3">
-        <v>822.89</v>
+        <v>377</v>
       </c>
       <c r="I12" s="3">
-        <v>856</v>
+        <v>465</v>
       </c>
       <c r="J12" s="3">
-        <v>889</v>
+        <v>573</v>
       </c>
       <c r="K12" s="3">
-        <v>921.98</v>
+        <v>706</v>
       </c>
       <c r="L12" s="3">
-        <v>957.19</v>
+        <v>871</v>
       </c>
       <c r="M12" s="3">
-        <v>992</v>
+        <v>1073</v>
       </c>
       <c r="N12" s="3">
-        <v>1028</v>
+        <v>1322</v>
       </c>
       <c r="O12" s="3">
-        <v>1063</v>
+        <v>1630</v>
       </c>
       <c r="P12" s="3">
-        <v>1098.03</v>
+        <v>2009</v>
       </c>
       <c r="Q12" s="3">
-        <v>1136</v>
+        <v>2475</v>
       </c>
       <c r="R12" s="3">
-        <v>1174</v>
+        <v>3051</v>
       </c>
       <c r="S12" s="3">
-        <v>1212.3699999999999</v>
+        <v>3760</v>
       </c>
       <c r="T12" s="3">
-        <v>1250</v>
+        <v>4634</v>
       </c>
       <c r="U12" s="3">
-        <v>1288.5999999999999</v>
+        <v>5710</v>
       </c>
       <c r="V12" s="3">
-        <v>18899.04</v>
+        <v>29817</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.2">
@@ -19231,67 +19331,67 @@
         <v>11</v>
       </c>
       <c r="B13" s="3">
-        <v>2952</v>
+        <v>506</v>
       </c>
       <c r="C13" s="3">
-        <v>3128</v>
+        <v>528</v>
       </c>
       <c r="D13" s="3">
-        <v>3303.14</v>
+        <v>552</v>
       </c>
       <c r="E13" s="3">
-        <v>3479</v>
+        <v>576</v>
       </c>
       <c r="F13" s="3">
-        <v>3654</v>
+        <v>601</v>
       </c>
       <c r="G13" s="3">
-        <v>3813.68</v>
+        <v>628</v>
       </c>
       <c r="H13" s="3">
-        <v>3973.17</v>
+        <v>655</v>
       </c>
       <c r="I13" s="3">
-        <v>4133</v>
+        <v>684</v>
       </c>
       <c r="J13" s="3">
-        <v>4292</v>
+        <v>714</v>
       </c>
       <c r="K13" s="3">
-        <v>4451.63</v>
+        <v>746</v>
       </c>
       <c r="L13" s="3">
-        <v>4621.63</v>
+        <v>779</v>
       </c>
       <c r="M13" s="3">
-        <v>4792</v>
+        <v>813</v>
       </c>
       <c r="N13" s="3">
-        <v>4962</v>
+        <v>849</v>
       </c>
       <c r="O13" s="3">
-        <v>5132</v>
+        <v>886</v>
       </c>
       <c r="P13" s="3">
-        <v>5301.64</v>
+        <v>925</v>
       </c>
       <c r="Q13" s="3">
-        <v>5486</v>
+        <v>966</v>
       </c>
       <c r="R13" s="3">
-        <v>5670</v>
+        <v>1008</v>
       </c>
       <c r="S13" s="3">
-        <v>5853.72</v>
+        <v>1052</v>
       </c>
       <c r="T13" s="3">
-        <v>6038</v>
+        <v>1099</v>
       </c>
       <c r="U13" s="3">
-        <v>6221.76</v>
+        <v>1147</v>
       </c>
       <c r="V13" s="3">
-        <v>91258.369999999981</v>
+        <v>15714</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.2">
@@ -19299,135 +19399,203 @@
         <v>12</v>
       </c>
       <c r="B14" s="3">
-        <v>978</v>
+        <v>180</v>
       </c>
       <c r="C14" s="3">
-        <v>1075</v>
+        <v>213</v>
       </c>
       <c r="D14" s="3">
-        <v>1182.8</v>
+        <v>252</v>
       </c>
       <c r="E14" s="3">
-        <v>1301</v>
+        <v>298</v>
       </c>
       <c r="F14" s="3">
-        <v>1431</v>
+        <v>352</v>
       </c>
       <c r="G14" s="3">
-        <v>1574.3</v>
+        <v>416</v>
       </c>
       <c r="H14" s="3">
-        <v>1731.74</v>
+        <v>492</v>
       </c>
       <c r="I14" s="3">
-        <v>1905</v>
+        <v>582</v>
       </c>
       <c r="J14" s="3">
-        <v>2095</v>
+        <v>688</v>
       </c>
       <c r="K14" s="3">
-        <v>2304.94</v>
+        <v>813</v>
       </c>
       <c r="L14" s="3">
-        <v>2535.4299999999998</v>
+        <v>897</v>
       </c>
       <c r="M14" s="3">
-        <v>2789</v>
+        <v>989</v>
       </c>
       <c r="N14" s="3">
-        <v>3068</v>
+        <v>1090</v>
       </c>
       <c r="O14" s="3">
-        <v>3375</v>
+        <v>1201</v>
       </c>
       <c r="P14" s="3">
-        <v>3712.13</v>
+        <v>1322</v>
       </c>
       <c r="Q14" s="3">
-        <v>4083</v>
+        <v>1464</v>
       </c>
       <c r="R14" s="3">
-        <v>4492</v>
+        <v>1620</v>
       </c>
       <c r="S14" s="3">
-        <v>4940.84</v>
+        <v>1792</v>
       </c>
       <c r="T14" s="3">
-        <v>5435</v>
+        <v>1981</v>
       </c>
       <c r="U14" s="3">
-        <v>5978.42</v>
+        <v>2189</v>
       </c>
       <c r="V14" s="3">
-        <v>55987.599999999991</v>
+        <v>18831</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="3">
+        <v>24</v>
+      </c>
+      <c r="C15" s="3">
+        <v>28</v>
+      </c>
+      <c r="D15" s="3">
+        <v>33</v>
+      </c>
+      <c r="E15" s="3">
+        <v>39</v>
+      </c>
+      <c r="F15" s="3">
+        <v>45</v>
+      </c>
+      <c r="G15" s="3">
+        <v>53</v>
+      </c>
+      <c r="H15" s="3">
+        <v>62</v>
+      </c>
+      <c r="I15" s="3">
+        <v>73</v>
+      </c>
+      <c r="J15" s="3">
+        <v>85</v>
+      </c>
+      <c r="K15" s="3">
+        <v>99</v>
+      </c>
+      <c r="L15" s="3">
+        <v>116</v>
+      </c>
+      <c r="M15" s="3">
+        <v>136</v>
+      </c>
+      <c r="N15" s="3">
+        <v>159</v>
+      </c>
+      <c r="O15" s="3">
+        <v>186</v>
+      </c>
+      <c r="P15" s="3">
+        <v>218</v>
+      </c>
+      <c r="Q15" s="3">
+        <v>255</v>
+      </c>
+      <c r="R15" s="3">
+        <v>298</v>
+      </c>
+      <c r="S15" s="3">
+        <v>348</v>
+      </c>
+      <c r="T15" s="3">
+        <v>407</v>
+      </c>
+      <c r="U15" s="3">
+        <v>476</v>
+      </c>
+      <c r="V15" s="3">
+        <v>3140</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="4">
-        <v>34443</v>
-      </c>
-      <c r="C15" s="4">
-        <v>36256</v>
-      </c>
-      <c r="D15" s="4">
-        <v>38339.26</v>
-      </c>
-      <c r="E15" s="4">
-        <v>40433</v>
-      </c>
-      <c r="F15" s="4">
-        <v>42541</v>
-      </c>
-      <c r="G15" s="4">
-        <v>44485.23</v>
-      </c>
-      <c r="H15" s="4">
-        <v>46444.479999999989</v>
-      </c>
-      <c r="I15" s="4">
-        <v>48420</v>
-      </c>
-      <c r="J15" s="4">
-        <v>50411</v>
-      </c>
-      <c r="K15" s="4">
-        <v>52423.130000000005</v>
-      </c>
-      <c r="L15" s="4">
-        <v>54567.270000000004</v>
-      </c>
-      <c r="M15" s="4">
-        <v>56739</v>
-      </c>
-      <c r="N15" s="4">
-        <v>58935</v>
-      </c>
-      <c r="O15" s="4">
-        <v>61158</v>
-      </c>
-      <c r="P15" s="4">
-        <v>63412.459999999992</v>
-      </c>
-      <c r="Q15" s="4">
-        <v>65856</v>
-      </c>
-      <c r="R15" s="4">
-        <v>68338</v>
-      </c>
-      <c r="S15" s="4">
-        <v>70860.210000000006</v>
-      </c>
-      <c r="T15" s="4">
-        <v>73426</v>
-      </c>
-      <c r="U15" s="4">
-        <v>76043.799999999988</v>
-      </c>
-      <c r="V15" s="4">
-        <v>1083531.8400000001</v>
+      <c r="B16" s="4">
+        <v>6814</v>
+      </c>
+      <c r="C16" s="4">
+        <v>7305</v>
+      </c>
+      <c r="D16" s="4">
+        <v>7845</v>
+      </c>
+      <c r="E16" s="4">
+        <v>8433</v>
+      </c>
+      <c r="F16" s="4">
+        <v>9078</v>
+      </c>
+      <c r="G16" s="4">
+        <v>9791</v>
+      </c>
+      <c r="H16" s="4">
+        <v>10576</v>
+      </c>
+      <c r="I16" s="4">
+        <v>11444</v>
+      </c>
+      <c r="J16" s="4">
+        <v>12401</v>
+      </c>
+      <c r="K16" s="4">
+        <v>13465</v>
+      </c>
+      <c r="L16" s="4">
+        <v>14540</v>
+      </c>
+      <c r="M16" s="4">
+        <v>15706</v>
+      </c>
+      <c r="N16" s="4">
+        <v>16974</v>
+      </c>
+      <c r="O16" s="4">
+        <v>18308</v>
+      </c>
+      <c r="P16" s="4">
+        <v>19781</v>
+      </c>
+      <c r="Q16" s="4">
+        <v>21362</v>
+      </c>
+      <c r="R16" s="4">
+        <v>23139</v>
+      </c>
+      <c r="S16" s="4">
+        <v>25139</v>
+      </c>
+      <c r="T16" s="4">
+        <v>27396</v>
+      </c>
+      <c r="U16" s="4">
+        <v>29956</v>
+      </c>
+      <c r="V16" s="4">
+        <v>309453</v>
       </c>
     </row>
   </sheetData>

</xml_diff>